<commit_message>
Feat: Added function of send e-mails after stop timer
</commit_message>
<xml_diff>
--- a/horasExtras.xlsx
+++ b/horasExtras.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoaoSimao\Documents\joao\EstudoRabbitMQ\GeradorPlanilhaHoras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6764D38-B6A9-4CE3-A547-F0480D67B32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A494033B-860B-4D9C-BC27-7FC39A6FF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,11 +73,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,60 +205,60 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" applyFill="1" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="2" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,21 +544,21 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1" style="11"/>
-    <col min="2" max="2" width="14.140625" customWidth="1" style="11"/>
-    <col min="3" max="3" width="20" customWidth="1" style="11"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1" style="11"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1" style="11"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1" style="15"/>
+    <col min="1" max="1" width="35.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="20" style="11" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="15" customWidth="1"/>
     <col min="7" max="7" width="63.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.25">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -570,7 +569,7 @@
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -583,13 +582,13 @@
       <c r="F2" s="12"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="19">
-        <f>SUM(F5:F1047615)</f>
-        <v>0.020844907407407406</v>
+        <f>SUM(F5:F1047597)</f>
+        <v>0</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="6"/>
@@ -597,7 +596,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
@@ -621,13 +620,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>